<commit_message>
Version 3.1 - Updated Sensor Programmer
Sensor programmer - wiring has been updated, resistor removed, and changed the diode. Maker Guide and BOM have been updated to reflect these changes. Typo in Maker Guide fixed.
</commit_message>
<xml_diff>
--- a/Documentation/Working_Documents/Twitch_Switch_BOM.xlsx
+++ b/Documentation/Working_Documents/Twitch_Switch_BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://neilsquiresoc.sharepoint.com/sites/MMCMounting/Shared Documents/Twitch Switch/Twitch-Switch/Documentation/Working_Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="880" documentId="11_DC0E2523FAFE28515E8D5C5A1D4A6B02C3B15AFA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{58C137CB-EB30-4276-89BA-6E4233B61AA6}"/>
+  <xr:revisionPtr revIDLastSave="893" documentId="11_DC0E2523FAFE28515E8D5C5A1D4A6B02C3B15AFA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CBD35E30-7F02-4158-B7CC-FC6F28043D1F}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="350">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="346">
   <si>
     <t>Total Cost</t>
   </si>
@@ -515,12 +515,6 @@
     <t>CP2102 Programmer</t>
   </si>
   <si>
-    <t>Schottky Diode</t>
-  </si>
-  <si>
-    <t>4.3 Ohm Resistor</t>
-  </si>
-  <si>
     <t>Solderless Breadboard</t>
   </si>
   <si>
@@ -614,9 +608,6 @@
     <t>455-1719-ND</t>
   </si>
   <si>
-    <t>SDM03MT40-FDICT-ND</t>
-  </si>
-  <si>
     <t>Twitch Controller</t>
   </si>
   <si>
@@ -740,9 +731,6 @@
     <t>D02</t>
   </si>
   <si>
-    <t>D03</t>
-  </si>
-  <si>
     <t>D04</t>
   </si>
   <si>
@@ -869,18 +857,6 @@
     <t>FIT0096</t>
   </si>
   <si>
-    <t>https://www.digikey.ca/en/products/detail/stackpole-electronics-inc/CF14JT4K30/1741423</t>
-  </si>
-  <si>
-    <t>CF14JT4K30CT-ND</t>
-  </si>
-  <si>
-    <t>CF14JT4K30</t>
-  </si>
-  <si>
-    <t>SDM03MT40-7-F</t>
-  </si>
-  <si>
     <t>1528-2233-ND</t>
   </si>
   <si>
@@ -912,9 +888,6 @@
   </si>
   <si>
     <t xml:space="preserve">https://www.canadarobotix.com/products/939 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.digikey.ca/en/products/detail/diodes-incorporated/SDM03MT40-7-F/814745?s=N4IgTCBcDaIMoBECyAGAzEgKgFhQWgDEEBJAYUzwDkEQBdAXyA </t>
   </si>
   <si>
     <t>https://www.amazon.ca/gp/product/B07D6LLX19</t>
@@ -1098,6 +1071,21 @@
   </si>
   <si>
     <t>Stereo cable should work fine</t>
+  </si>
+  <si>
+    <t>IN4002 Diode</t>
+  </si>
+  <si>
+    <t>Diotec Semiconductor</t>
+  </si>
+  <si>
+    <t>1N4002</t>
+  </si>
+  <si>
+    <t>4878-1N4002CT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.ca/en/products/detail/diotec-semiconductor/1N4002/13164611 </t>
   </si>
 </sst>
 </file>
@@ -1542,7 +1530,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="5" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="8" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1555,6 +1542,7 @@
     <xf numFmtId="44" fontId="0" fillId="11" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="11" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1849,11 +1837,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R106"/>
+  <dimension ref="A1:R105"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P40" sqref="P40"/>
+      <pane ySplit="3" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1894,8 +1882,8 @@
       <c r="B2" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="66">
-        <v>3</v>
+      <c r="C2" s="65">
+        <v>3.1</v>
       </c>
       <c r="E2" t="s">
         <v>11</v>
@@ -1905,19 +1893,19 @@
       </c>
       <c r="H2" s="10"/>
       <c r="J2" s="6">
-        <f>SUM(J48:J57)</f>
+        <f>SUM(J47:J56)</f>
         <v>56</v>
       </c>
       <c r="M2" s="20">
-        <f>SUM(M6:M37,M40:M44,M48:M57)</f>
-        <v>197.94693091666664</v>
+        <f>SUM(M6:M36,M39:M43,M47:M56)</f>
+        <v>197.28693091666665</v>
       </c>
       <c r="N2" s="5">
-        <f>SUM(N6:N57)</f>
-        <v>373.72503999999986</v>
+        <f>SUM(N6:N56)</f>
+        <v>373.06503999999984</v>
       </c>
       <c r="O2" s="21">
-        <f>SUM(O48:O57)</f>
+        <f>SUM(O47:O56)</f>
         <v>0.25972222222222224</v>
       </c>
     </row>
@@ -1970,7 +1958,7 @@
         <v>22</v>
       </c>
       <c r="R3" s="7" t="s">
-        <v>343</v>
+        <v>334</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1997,7 +1985,7 @@
     </row>
     <row r="5" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="72" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B5" s="72"/>
       <c r="C5" s="72"/>
@@ -2021,7 +2009,7 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B6" t="s">
         <v>73</v>
@@ -2068,7 +2056,7 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B7" t="s">
         <v>74</v>
@@ -2115,7 +2103,7 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B8" t="s">
         <v>75</v>
@@ -2162,7 +2150,7 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B9" t="s">
         <v>76</v>
@@ -2209,7 +2197,7 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B10" t="s">
         <v>77</v>
@@ -2256,7 +2244,7 @@
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B11" t="s">
         <v>78</v>
@@ -2303,7 +2291,7 @@
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B12" t="s">
         <v>79</v>
@@ -2350,7 +2338,7 @@
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B13" t="s">
         <v>80</v>
@@ -2397,19 +2385,19 @@
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B14" t="s">
-        <v>345</v>
+        <v>336</v>
       </c>
       <c r="C14" t="s">
-        <v>344</v>
+        <v>335</v>
       </c>
       <c r="E14" t="s">
-        <v>301</v>
+        <v>292</v>
       </c>
       <c r="G14" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="I14">
         <v>24</v>
@@ -2433,12 +2421,12 @@
         <v>9.3000000000000007</v>
       </c>
       <c r="P14" s="25" t="s">
-        <v>302</v>
+        <v>293</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B15" t="s">
         <v>81</v>
@@ -2486,23 +2474,23 @@
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B16" s="37" t="s">
         <v>82</v>
       </c>
       <c r="C16" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
       <c r="D16" s="26"/>
       <c r="E16" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="F16" t="s">
         <v>63</v>
       </c>
       <c r="G16" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="H16" s="37"/>
       <c r="I16">
@@ -2527,23 +2515,23 @@
         <v>5.5</v>
       </c>
       <c r="P16" s="8" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="R16" t="s">
-        <v>347</v>
+        <v>338</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B17" s="37"/>
       <c r="C17" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="D17" s="26"/>
       <c r="E17" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="F17">
         <v>2886</v>
@@ -2552,7 +2540,7 @@
         <v>72</v>
       </c>
       <c r="H17" s="37" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="I17">
         <v>1</v>
@@ -2576,28 +2564,28 @@
         <v>1.36</v>
       </c>
       <c r="P17" s="25" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B18" s="37" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
       <c r="C18" s="38" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="D18" s="26"/>
       <c r="E18" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="F18" t="s">
-        <v>298</v>
+        <v>289</v>
       </c>
       <c r="G18" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="H18" s="37">
         <v>2528</v>
@@ -2624,25 +2612,25 @@
         <v>14.99</v>
       </c>
       <c r="P18" s="8" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B19" s="37" t="s">
-        <v>340</v>
+        <v>331</v>
       </c>
       <c r="C19" t="s">
-        <v>341</v>
+        <v>332</v>
       </c>
       <c r="D19" s="26"/>
       <c r="E19" t="s">
-        <v>339</v>
+        <v>330</v>
       </c>
       <c r="G19" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="H19" s="37"/>
       <c r="I19">
@@ -2668,32 +2656,32 @@
         <v>8.99</v>
       </c>
       <c r="P19" s="25" t="s">
-        <v>338</v>
+        <v>329</v>
       </c>
       <c r="Q19" t="s">
-        <v>346</v>
+        <v>337</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B20" s="37"/>
       <c r="C20" s="38" t="s">
-        <v>334</v>
+        <v>325</v>
       </c>
       <c r="D20" s="26"/>
       <c r="E20" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="F20" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="G20" t="s">
         <v>72</v>
       </c>
       <c r="H20" s="37" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="I20">
         <v>2</v>
@@ -2717,29 +2705,29 @@
         <v>26.33</v>
       </c>
       <c r="P20" s="25" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="21" spans="1:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="18" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B21" s="39"/>
       <c r="C21" s="40" t="s">
-        <v>335</v>
+        <v>326</v>
       </c>
       <c r="D21" s="41"/>
       <c r="E21" s="40" t="s">
-        <v>336</v>
+        <v>327</v>
       </c>
       <c r="F21" s="40" t="s">
-        <v>295</v>
+        <v>286</v>
       </c>
       <c r="G21" s="40" t="s">
-        <v>336</v>
+        <v>327</v>
       </c>
       <c r="H21" s="40" t="s">
-        <v>295</v>
+        <v>286</v>
       </c>
       <c r="I21" s="18">
         <v>4</v>
@@ -2764,14 +2752,14 @@
       </c>
       <c r="O21" s="18"/>
       <c r="P21" s="57" t="s">
-        <v>297</v>
+        <v>288</v>
       </c>
       <c r="Q21" s="18"/>
       <c r="R21" s="18"/>
     </row>
     <row r="22" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="73" t="s">
-        <v>320</v>
+        <v>311</v>
       </c>
       <c r="B22" s="73"/>
       <c r="C22" s="73"/>
@@ -2795,7 +2783,7 @@
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="B23" t="s">
         <v>143</v>
@@ -2813,7 +2801,7 @@
         <v>72</v>
       </c>
       <c r="H23" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="I23">
         <f>$I$22*1</f>
@@ -2838,28 +2826,28 @@
         <v>0.75</v>
       </c>
       <c r="P23" s="25" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="B24" s="37" t="s">
         <v>79</v>
       </c>
       <c r="C24" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
       <c r="D24" s="26"/>
       <c r="E24" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="F24" t="s">
         <v>63</v>
       </c>
       <c r="G24" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="H24" s="37"/>
       <c r="I24">
@@ -2885,31 +2873,31 @@
         <v>11</v>
       </c>
       <c r="P24" s="8" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="R24" t="s">
-        <v>348</v>
+        <v>339</v>
       </c>
     </row>
     <row r="25" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="18" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B25" s="39" t="s">
-        <v>299</v>
+        <v>290</v>
       </c>
       <c r="C25" s="40" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="D25" s="41"/>
       <c r="E25" s="18" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="F25" s="18">
         <v>930</v>
       </c>
       <c r="G25" s="18" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="H25" s="39"/>
       <c r="I25" s="18">
@@ -2936,14 +2924,14 @@
       </c>
       <c r="O25" s="18"/>
       <c r="P25" s="57" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
       <c r="Q25" s="18"/>
       <c r="R25" s="18"/>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="74" t="s">
-        <v>305</v>
+        <v>296</v>
       </c>
       <c r="B26" s="74"/>
       <c r="C26" s="74"/>
@@ -2963,99 +2951,99 @@
       <c r="Q26" s="28"/>
       <c r="R26" s="28"/>
     </row>
-    <row r="27" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B27" s="37" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="C27" s="38" t="s">
-        <v>314</v>
+        <v>305</v>
       </c>
       <c r="D27" s="26"/>
       <c r="E27" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="F27" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="G27" t="s">
         <v>72</v>
       </c>
       <c r="H27" s="37" t="s">
-        <v>317</v>
-      </c>
-      <c r="I27" s="18">
-        <v>1</v>
-      </c>
-      <c r="J27" s="18">
-        <v>1</v>
-      </c>
-      <c r="K27" s="42">
+        <v>308</v>
+      </c>
+      <c r="I27">
+        <v>1</v>
+      </c>
+      <c r="J27">
+        <v>1</v>
+      </c>
+      <c r="K27" s="23">
         <f>IF(I27&gt;0,CEILING(I27/J27,1),0)</f>
         <v>1</v>
       </c>
-      <c r="L27" s="61">
+      <c r="L27" s="71">
         <v>3.57</v>
       </c>
-      <c r="M27" s="43">
+      <c r="M27" s="24">
         <f>IF(I27&gt;0,L27/J27*I27,0)</f>
         <v>3.57</v>
       </c>
-      <c r="N27" s="43">
+      <c r="N27" s="24">
         <f>K27*L27</f>
         <v>3.57</v>
       </c>
       <c r="P27" s="60" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="28" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B28" s="37" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
       <c r="C28" s="38" t="s">
-        <v>309</v>
+        <v>300</v>
       </c>
       <c r="D28" s="26"/>
       <c r="E28" t="s">
-        <v>310</v>
+        <v>301</v>
       </c>
       <c r="F28" t="s">
-        <v>311</v>
+        <v>302</v>
       </c>
       <c r="G28" t="s">
         <v>72</v>
       </c>
       <c r="H28" s="37" t="s">
-        <v>312</v>
-      </c>
-      <c r="I28" s="18">
-        <v>1</v>
-      </c>
-      <c r="J28" s="18">
-        <v>1</v>
-      </c>
-      <c r="K28" s="42">
+        <v>303</v>
+      </c>
+      <c r="I28">
+        <v>1</v>
+      </c>
+      <c r="J28">
+        <v>1</v>
+      </c>
+      <c r="K28" s="23">
         <f>IF(I28&gt;0,CEILING(I28/J28,1),0)</f>
         <v>1</v>
       </c>
-      <c r="L28" s="58">
+      <c r="L28" s="36">
         <v>2.2400000000000002</v>
       </c>
-      <c r="M28" s="43">
+      <c r="M28" s="24">
         <f>IF(I28&gt;0,L28/J28*I28,0)</f>
         <v>2.2400000000000002</v>
       </c>
-      <c r="N28" s="43">
+      <c r="N28" s="24">
         <f>K28*L28</f>
         <v>2.2400000000000002</v>
       </c>
       <c r="P28" s="60" t="s">
-        <v>313</v>
+        <v>304</v>
       </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="74" t="s">
-        <v>306</v>
+        <v>297</v>
       </c>
       <c r="B29" s="74"/>
       <c r="C29" s="74"/>
@@ -3077,22 +3065,22 @@
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
       <c r="C30" s="38" t="s">
-        <v>321</v>
+        <v>312</v>
       </c>
       <c r="E30" t="s">
-        <v>322</v>
+        <v>313</v>
       </c>
       <c r="F30" t="s">
-        <v>323</v>
+        <v>314</v>
       </c>
       <c r="G30" t="s">
         <v>72</v>
       </c>
       <c r="H30" t="s">
-        <v>324</v>
+        <v>315</v>
       </c>
       <c r="I30">
         <v>3</v>
@@ -3115,12 +3103,12 @@
         <v>12.11</v>
       </c>
       <c r="P30" s="8" t="s">
-        <v>326</v>
+        <v>317</v>
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="74" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B31" s="74"/>
       <c r="C31" s="74"/>
@@ -3142,17 +3130,17 @@
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="C32" s="26" t="s">
         <v>158</v>
       </c>
       <c r="D32" s="26"/>
       <c r="E32" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="G32" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="H32" s="31"/>
       <c r="I32">
@@ -3162,7 +3150,7 @@
         <v>2</v>
       </c>
       <c r="K32" s="23">
-        <f t="shared" ref="K32:K37" si="6">IF(I32&gt;0,CEILING(I32/J32,1),0)</f>
+        <f t="shared" ref="K32:K36" si="6">IF(I32&gt;0,CEILING(I32/J32,1),0)</f>
         <v>1</v>
       </c>
       <c r="L32" s="9">
@@ -3177,28 +3165,28 @@
         <v>9.98</v>
       </c>
       <c r="P32" s="8" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C33" s="26" t="s">
-        <v>159</v>
+        <v>341</v>
       </c>
       <c r="D33" s="26"/>
       <c r="E33" t="s">
-        <v>104</v>
+        <v>342</v>
       </c>
       <c r="F33" t="s">
-        <v>280</v>
+        <v>343</v>
       </c>
       <c r="G33" t="s">
         <v>72</v>
       </c>
       <c r="H33" t="s">
-        <v>192</v>
+        <v>344</v>
       </c>
       <c r="I33">
         <v>1</v>
@@ -3211,39 +3199,39 @@
         <v>1</v>
       </c>
       <c r="L33" s="9">
-        <v>0.66</v>
+        <v>0.15</v>
       </c>
       <c r="M33" s="24">
-        <f t="shared" ref="M33:M37" si="7">IF(I33&gt;0,L33/J33*I33,0)</f>
-        <v>0.66</v>
+        <f t="shared" ref="M33:M36" si="7">IF(I33&gt;0,L33/J33*I33,0)</f>
+        <v>0.15</v>
       </c>
       <c r="N33" s="24">
-        <f t="shared" ref="N33:N37" si="8">K33*L33</f>
-        <v>0.66</v>
+        <f t="shared" ref="N33:N36" si="8">K33*L33</f>
+        <v>0.15</v>
       </c>
       <c r="P33" s="8" t="s">
-        <v>292</v>
+        <v>345</v>
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="C34" s="26" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D34" s="26"/>
       <c r="E34" t="s">
-        <v>108</v>
+        <v>271</v>
       </c>
       <c r="F34" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="G34" t="s">
         <v>72</v>
       </c>
-      <c r="H34" s="26" t="s">
-        <v>278</v>
+      <c r="H34" t="s">
+        <v>269</v>
       </c>
       <c r="I34">
         <v>1</v>
@@ -3256,247 +3244,238 @@
         <v>1</v>
       </c>
       <c r="L34" s="9">
-        <v>0.15</v>
+        <v>4.43</v>
       </c>
       <c r="M34" s="24">
         <f t="shared" si="7"/>
-        <v>0.15</v>
+        <v>4.43</v>
       </c>
       <c r="N34" s="24">
         <f t="shared" si="8"/>
-        <v>0.15</v>
+        <v>4.43</v>
       </c>
       <c r="P34" s="8" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C35" s="26" t="s">
-        <v>161</v>
+        <v>228</v>
       </c>
       <c r="D35" s="26"/>
       <c r="E35" t="s">
-        <v>275</v>
-      </c>
-      <c r="F35" t="s">
-        <v>276</v>
+        <v>50</v>
+      </c>
+      <c r="F35">
+        <v>1953</v>
       </c>
       <c r="G35" t="s">
         <v>72</v>
       </c>
-      <c r="H35" t="s">
+      <c r="H35" s="26" t="s">
         <v>273</v>
       </c>
       <c r="I35">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="J35">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="K35" s="23">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="L35" s="9">
-        <v>4.43</v>
+        <v>2.79</v>
       </c>
       <c r="M35" s="24">
         <f t="shared" si="7"/>
-        <v>4.43</v>
+        <v>0.69750000000000001</v>
       </c>
       <c r="N35" s="24">
         <f t="shared" si="8"/>
-        <v>4.43</v>
+        <v>2.79</v>
       </c>
       <c r="P35" s="8" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="18" t="s">
+        <v>233</v>
+      </c>
+      <c r="B36" s="18"/>
+      <c r="C36" s="41" t="s">
+        <v>227</v>
+      </c>
+      <c r="D36" s="41"/>
+      <c r="E36" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="F36" s="18">
+        <v>1956</v>
+      </c>
+      <c r="G36" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="H36" s="41" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>236</v>
-      </c>
-      <c r="C36" s="26" t="s">
-        <v>231</v>
-      </c>
-      <c r="D36" s="26"/>
-      <c r="E36" t="s">
-        <v>50</v>
-      </c>
-      <c r="F36">
-        <v>1953</v>
-      </c>
-      <c r="G36" t="s">
-        <v>72</v>
-      </c>
-      <c r="H36" s="26" t="s">
-        <v>281</v>
-      </c>
-      <c r="I36">
-        <v>5</v>
-      </c>
-      <c r="J36">
+      <c r="I36" s="18">
+        <v>2</v>
+      </c>
+      <c r="J36" s="18">
         <v>20</v>
       </c>
-      <c r="K36" s="23">
+      <c r="K36" s="42">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="L36" s="9">
+      <c r="L36" s="49">
         <v>2.79</v>
       </c>
-      <c r="M36" s="24">
+      <c r="M36" s="43">
         <f t="shared" si="7"/>
-        <v>0.69750000000000001</v>
-      </c>
-      <c r="N36" s="24">
+        <v>0.27900000000000003</v>
+      </c>
+      <c r="N36" s="43">
         <f t="shared" si="8"/>
         <v>2.79</v>
       </c>
-      <c r="P36" s="8" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="37" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="18" t="s">
-        <v>237</v>
-      </c>
-      <c r="B37" s="18"/>
-      <c r="C37" s="41" t="s">
-        <v>230</v>
-      </c>
-      <c r="D37" s="41"/>
-      <c r="E37" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="F37" s="18">
-        <v>1956</v>
-      </c>
-      <c r="G37" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="H37" s="41" t="s">
-        <v>282</v>
-      </c>
-      <c r="I37" s="18">
-        <v>2</v>
-      </c>
-      <c r="J37" s="18">
+      <c r="O36" s="18"/>
+      <c r="P36" s="50" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="48" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D38" s="7"/>
+      <c r="E38" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F38" s="7"/>
+      <c r="G38" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H38" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="I38" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="J38" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="K38" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="L38" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="K37" s="42">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="L37" s="49">
-        <v>2.79</v>
-      </c>
-      <c r="M37" s="43">
-        <f t="shared" si="7"/>
-        <v>0.27900000000000003</v>
-      </c>
-      <c r="N37" s="43">
-        <f t="shared" si="8"/>
-        <v>2.79</v>
-      </c>
-      <c r="O37" s="18"/>
-      <c r="P37" s="50" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="38" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="48" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="39" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C39" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D39" s="7"/>
-      <c r="E39" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F39" s="7"/>
-      <c r="G39" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="H39" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="I39" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="J39" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="K39" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="L39" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="M39" s="7" t="s">
+      <c r="M38" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="N39" s="7" t="s">
+      <c r="N38" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="O39" s="7"/>
-      <c r="P39" s="7" t="s">
+      <c r="O38" s="7"/>
+      <c r="P38" s="7" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>196</v>
+      </c>
+      <c r="B39" t="s">
+        <v>25</v>
+      </c>
+      <c r="C39" t="s">
+        <v>175</v>
+      </c>
+      <c r="E39" t="s">
+        <v>26</v>
+      </c>
+      <c r="I39">
+        <v>1</v>
+      </c>
+      <c r="J39">
+        <v>5</v>
+      </c>
+      <c r="K39">
+        <f t="shared" ref="K39:K43" si="9">IF(I39&gt;0,CEILING(I39/J39,1),0)</f>
+        <v>1</v>
+      </c>
+      <c r="L39">
+        <v>5</v>
+      </c>
+      <c r="M39">
+        <f>IF(I39&gt;0,L39/J39*I39,0)</f>
+        <v>1</v>
+      </c>
+      <c r="N39">
+        <f t="shared" ref="N39:N43" si="10">K39*L39</f>
+        <v>5</v>
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>199</v>
+        <v>310</v>
       </c>
       <c r="B40" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="C40" t="s">
-        <v>177</v>
+        <v>323</v>
       </c>
       <c r="E40" t="s">
         <v>26</v>
       </c>
       <c r="I40">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J40">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="K40">
-        <f t="shared" ref="K40:K44" si="9">IF(I40&gt;0,CEILING(I40/J40,1),0)</f>
-        <v>1</v>
-      </c>
-      <c r="L40">
-        <v>5</v>
-      </c>
-      <c r="M40">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="L40" s="64">
+        <f>88.71*1.36/10</f>
+        <v>12.06456</v>
+      </c>
+      <c r="M40" s="63">
         <f>IF(I40&gt;0,L40/J40*I40,0)</f>
-        <v>1</v>
-      </c>
-      <c r="N40">
-        <f t="shared" ref="N40:N44" si="10">K40*L40</f>
-        <v>5</v>
+        <v>2.4129119999999999</v>
+      </c>
+      <c r="N40" s="63">
+        <f t="shared" si="10"/>
+        <v>12.06456</v>
       </c>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>319</v>
+        <v>244</v>
       </c>
       <c r="B41" t="s">
-        <v>35</v>
+        <v>322</v>
       </c>
       <c r="C41" t="s">
-        <v>332</v>
+        <v>324</v>
       </c>
       <c r="E41" t="s">
         <v>26</v>
@@ -3508,56 +3487,55 @@
         <v>15</v>
       </c>
       <c r="K41">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="L41" s="65">
-        <f>88.71*1.36/10</f>
-        <v>12.06456</v>
-      </c>
-      <c r="M41" s="64">
-        <f>IF(I41&gt;0,L41/J41*I41,0)</f>
-        <v>2.4129119999999999</v>
-      </c>
-      <c r="N41" s="64">
-        <f t="shared" si="10"/>
-        <v>12.06456</v>
-      </c>
-    </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>248</v>
-      </c>
-      <c r="B42" t="s">
-        <v>331</v>
-      </c>
-      <c r="C42" t="s">
-        <v>333</v>
-      </c>
-      <c r="E42" t="s">
-        <v>26</v>
-      </c>
-      <c r="I42">
-        <v>3</v>
-      </c>
-      <c r="J42">
-        <v>15</v>
-      </c>
-      <c r="K42">
-        <f t="shared" ref="K42" si="11">IF(I42&gt;0,CEILING(I42/J42,1),0)</f>
-        <v>1</v>
-      </c>
-      <c r="L42" s="65">
+        <f t="shared" ref="K41" si="11">IF(I41&gt;0,CEILING(I41/J41,1),0)</f>
+        <v>1</v>
+      </c>
+      <c r="L41" s="64">
         <f>908.68*1.36/10</f>
         <v>123.58048000000001</v>
       </c>
-      <c r="M42" s="64">
+      <c r="M41" s="63">
+        <f>IF(I41&gt;0,L41/J41*I41,0)</f>
+        <v>24.716096000000004</v>
+      </c>
+      <c r="N41" s="63">
+        <f t="shared" ref="N41" si="12">K41*L41</f>
+        <v>123.58048000000001</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>27</v>
+      </c>
+      <c r="C42" t="s">
+        <v>28</v>
+      </c>
+      <c r="D42" t="s">
+        <v>29</v>
+      </c>
+      <c r="I42">
+        <v>1</v>
+      </c>
+      <c r="J42">
+        <v>5</v>
+      </c>
+      <c r="K42">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="L42">
+        <v>25</v>
+      </c>
+      <c r="M42">
         <f>IF(I42&gt;0,L42/J42*I42,0)</f>
-        <v>24.716096000000004</v>
-      </c>
-      <c r="N42" s="64">
-        <f t="shared" ref="N42" si="12">K42*L42</f>
-        <v>123.58048000000001</v>
+        <v>5</v>
+      </c>
+      <c r="N42">
+        <f t="shared" si="10"/>
+        <v>25</v>
+      </c>
+      <c r="Q42" t="s">
+        <v>328</v>
       </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.25">
@@ -3565,139 +3543,133 @@
         <v>27</v>
       </c>
       <c r="C43" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D43" t="s">
         <v>29</v>
       </c>
       <c r="I43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J43">
         <v>5</v>
       </c>
       <c r="K43">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L43">
         <v>25</v>
       </c>
       <c r="M43">
         <f>IF(I43&gt;0,L43/J43*I43,0)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="N43">
         <f t="shared" si="10"/>
-        <v>25</v>
-      </c>
-      <c r="Q43" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B44" t="s">
-        <v>27</v>
-      </c>
-      <c r="C44" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="18"/>
+      <c r="B44" s="18"/>
+      <c r="C44" s="18"/>
+      <c r="D44" s="18"/>
+      <c r="E44" s="18"/>
+      <c r="F44" s="18"/>
+      <c r="G44" s="18"/>
+      <c r="H44" s="18"/>
+      <c r="I44" s="18"/>
+      <c r="J44" s="18"/>
+      <c r="K44" s="18"/>
+      <c r="L44" s="18"/>
+      <c r="M44" s="53"/>
+      <c r="N44" s="53"/>
+      <c r="O44" s="18"/>
+      <c r="P44" s="18"/>
+    </row>
+    <row r="45" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B45" s="51" t="s">
+        <v>5</v>
+      </c>
+      <c r="C45" s="52">
         <v>30</v>
       </c>
-      <c r="D44" t="s">
-        <v>29</v>
-      </c>
-      <c r="I44">
-        <v>0</v>
-      </c>
-      <c r="J44">
-        <v>5</v>
-      </c>
-      <c r="K44">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="L44">
-        <v>25</v>
-      </c>
-      <c r="M44">
-        <f>IF(I44&gt;0,L44/J44*I44,0)</f>
-        <v>0</v>
-      </c>
-      <c r="N44">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="18"/>
-      <c r="B45" s="18"/>
-      <c r="C45" s="18"/>
-      <c r="D45" s="18"/>
-      <c r="E45" s="18"/>
-      <c r="F45" s="18"/>
-      <c r="G45" s="18"/>
-      <c r="H45" s="18"/>
-      <c r="I45" s="18"/>
-      <c r="J45" s="18"/>
-      <c r="K45" s="18"/>
-      <c r="L45" s="18"/>
-      <c r="M45" s="53"/>
-      <c r="N45" s="53"/>
-      <c r="O45" s="18"/>
-      <c r="P45" s="18"/>
+      <c r="L45" s="9"/>
+      <c r="M45" s="16"/>
+      <c r="N45" s="16"/>
+      <c r="O45" s="20"/>
     </row>
     <row r="46" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="51" t="s">
-        <v>5</v>
-      </c>
-      <c r="C46" s="52">
-        <v>30</v>
-      </c>
-      <c r="L46" s="9"/>
-      <c r="M46" s="16"/>
-      <c r="N46" s="16"/>
-      <c r="O46" s="20"/>
-    </row>
-    <row r="47" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="7" t="s">
+      <c r="B46" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C47" s="17" t="s">
+      <c r="C46" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="D47" s="7"/>
-      <c r="E47" s="7"/>
-      <c r="F47" s="7"/>
-      <c r="G47" s="7"/>
-      <c r="H47" s="7"/>
-      <c r="I47" s="7" t="s">
+      <c r="D46" s="7"/>
+      <c r="E46" s="7"/>
+      <c r="F46" s="7"/>
+      <c r="G46" s="7"/>
+      <c r="H46" s="7"/>
+      <c r="I46" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="J47" s="7" t="s">
+      <c r="J46" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="K47" s="7"/>
-      <c r="L47" s="14" t="s">
+      <c r="K46" s="7"/>
+      <c r="L46" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="M47" s="7" t="s">
+      <c r="M46" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="N47" s="7" t="s">
+      <c r="N46" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="O47" s="7" t="s">
+      <c r="O46" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="P47" s="7" t="s">
+      <c r="P46" s="7" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>212</v>
+      </c>
+      <c r="C47" t="s">
+        <v>193</v>
+      </c>
+      <c r="I47">
+        <v>1</v>
+      </c>
+      <c r="J47">
+        <v>20</v>
+      </c>
+      <c r="L47" s="32">
+        <f>J47/1000*$C$45</f>
+        <v>0.6</v>
+      </c>
+      <c r="M47" s="32">
+        <f>L47</f>
+        <v>0.6</v>
+      </c>
+      <c r="N47" s="32">
+        <f>L47</f>
+        <v>0.6</v>
+      </c>
+      <c r="O47" s="33">
+        <v>9.0972222222222218E-2</v>
       </c>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="C48" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="I48">
         <v>1</v>
@@ -3706,59 +3678,59 @@
         <v>20</v>
       </c>
       <c r="L48" s="32">
-        <f>J48/1000*$C$46</f>
+        <f t="shared" ref="L48:L54" si="13">J48/1000*$C$45</f>
         <v>0.6</v>
       </c>
       <c r="M48" s="32">
-        <f>L48</f>
+        <f t="shared" ref="M48:M54" si="14">L48</f>
         <v>0.6</v>
       </c>
       <c r="N48" s="32">
-        <f>L48</f>
+        <f t="shared" ref="N48:N54" si="15">L48</f>
         <v>0.6</v>
       </c>
       <c r="O48" s="33">
-        <v>9.0972222222222218E-2</v>
+        <v>9.2361111111111116E-2</v>
       </c>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C49" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="I49">
         <v>1</v>
       </c>
       <c r="J49">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="L49" s="32">
-        <f t="shared" ref="L49:L55" si="13">J49/1000*$C$46</f>
-        <v>0.6</v>
+        <f t="shared" si="13"/>
+        <v>0.03</v>
       </c>
       <c r="M49" s="32">
-        <f t="shared" ref="M49:M55" si="14">L49</f>
-        <v>0.6</v>
+        <f t="shared" si="14"/>
+        <v>0.03</v>
       </c>
       <c r="N49" s="32">
-        <f t="shared" ref="N49:N55" si="15">L49</f>
-        <v>0.6</v>
+        <f t="shared" si="15"/>
+        <v>0.03</v>
       </c>
       <c r="O49" s="33">
-        <v>9.2361111111111116E-2</v>
+        <v>3.472222222222222E-3</v>
       </c>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C50" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="I50">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J50">
         <v>1</v>
@@ -3776,73 +3748,73 @@
         <v>0.03</v>
       </c>
       <c r="O50" s="33">
-        <v>3.472222222222222E-3</v>
+        <v>9.7222222222222224E-3</v>
       </c>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>217</v>
+        <v>236</v>
       </c>
       <c r="C51" t="s">
-        <v>198</v>
+        <v>240</v>
       </c>
       <c r="I51">
         <v>3</v>
       </c>
       <c r="J51">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="L51" s="32">
         <f t="shared" si="13"/>
-        <v>0.03</v>
+        <v>0.15</v>
       </c>
       <c r="M51" s="32">
         <f t="shared" si="14"/>
-        <v>0.03</v>
+        <v>0.15</v>
       </c>
       <c r="N51" s="32">
         <f t="shared" si="15"/>
-        <v>0.03</v>
+        <v>0.15</v>
       </c>
       <c r="O51" s="33">
-        <v>9.7222222222222224E-3</v>
+        <v>2.361111111111111E-2</v>
       </c>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="C52" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="I52">
+        <v>1</v>
+      </c>
+      <c r="J52">
         <v>3</v>
-      </c>
-      <c r="J52">
-        <v>5</v>
       </c>
       <c r="L52" s="32">
         <f t="shared" si="13"/>
-        <v>0.15</v>
+        <v>0.09</v>
       </c>
       <c r="M52" s="32">
         <f t="shared" si="14"/>
-        <v>0.15</v>
+        <v>0.09</v>
       </c>
       <c r="N52" s="32">
         <f t="shared" si="15"/>
-        <v>0.15</v>
+        <v>0.09</v>
       </c>
       <c r="O52" s="33">
-        <v>2.361111111111111E-2</v>
+        <v>1.3194444444444444E-2</v>
       </c>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="C53" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="I53">
         <v>1</v>
@@ -3868,10 +3840,10 @@
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="C54" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="I54">
         <v>1</v>
@@ -3896,107 +3868,119 @@
       </c>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>243</v>
-      </c>
-      <c r="C55" t="s">
-        <v>247</v>
-      </c>
-      <c r="I55">
-        <v>1</v>
-      </c>
-      <c r="J55">
-        <v>3</v>
-      </c>
-      <c r="L55" s="32">
-        <f t="shared" si="13"/>
-        <v>0.09</v>
-      </c>
-      <c r="M55" s="32">
-        <f t="shared" si="14"/>
-        <v>0.09</v>
-      </c>
-      <c r="N55" s="32">
-        <f t="shared" si="15"/>
-        <v>0.09</v>
-      </c>
-      <c r="O55" s="33">
-        <v>1.3194444444444444E-2</v>
-      </c>
-    </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="L56" s="67"/>
-      <c r="M56" s="67"/>
-      <c r="N56" s="67"/>
-      <c r="O56" s="33"/>
-    </row>
-    <row r="57" spans="1:16" s="71" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="68"/>
-      <c r="B57" s="68"/>
-      <c r="C57" s="68"/>
-      <c r="D57" s="68"/>
-      <c r="E57" s="68"/>
-      <c r="F57" s="68"/>
-      <c r="G57" s="68"/>
-      <c r="H57" s="68"/>
-      <c r="I57" s="68"/>
-      <c r="J57" s="68"/>
-      <c r="K57" s="68"/>
-      <c r="L57" s="69">
-        <f>J57/1000*$C$46</f>
+      <c r="L55" s="66"/>
+      <c r="M55" s="66"/>
+      <c r="N55" s="66"/>
+      <c r="O55" s="33"/>
+    </row>
+    <row r="56" spans="1:16" s="70" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="67"/>
+      <c r="B56" s="67"/>
+      <c r="C56" s="67"/>
+      <c r="D56" s="67"/>
+      <c r="E56" s="67"/>
+      <c r="F56" s="67"/>
+      <c r="G56" s="67"/>
+      <c r="H56" s="67"/>
+      <c r="I56" s="67"/>
+      <c r="J56" s="67"/>
+      <c r="K56" s="67"/>
+      <c r="L56" s="68">
+        <f>J56/1000*$C$45</f>
         <v>0</v>
       </c>
-      <c r="M57" s="69">
-        <f t="shared" ref="M57" si="16">L57</f>
+      <c r="M56" s="68">
+        <f t="shared" ref="M56" si="16">L56</f>
         <v>0</v>
       </c>
-      <c r="N57" s="69">
-        <f t="shared" ref="N57" si="17">L57</f>
+      <c r="N56" s="68">
+        <f t="shared" ref="N56" si="17">L56</f>
         <v>0</v>
       </c>
-      <c r="O57" s="70"/>
-      <c r="P57" s="68"/>
+      <c r="O56" s="69"/>
+      <c r="P56" s="67"/>
+    </row>
+    <row r="57" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B57" s="54" t="s">
+        <v>33</v>
+      </c>
+      <c r="C57" s="15"/>
+      <c r="D57" s="15"/>
+      <c r="E57" s="15"/>
+      <c r="F57" s="15"/>
+      <c r="G57" s="15"/>
+      <c r="H57" s="15"/>
+      <c r="I57" s="15"/>
+      <c r="J57" s="15"/>
+      <c r="K57" s="15"/>
+      <c r="L57" s="15"/>
+      <c r="M57" s="15"/>
+      <c r="N57" s="15"/>
+      <c r="O57" s="15"/>
+      <c r="P57" s="15"/>
     </row>
     <row r="58" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="54" t="s">
-        <v>33</v>
-      </c>
-      <c r="C58" s="15"/>
-      <c r="D58" s="15"/>
-      <c r="E58" s="15"/>
-      <c r="F58" s="15"/>
-      <c r="G58" s="15"/>
-      <c r="H58" s="15"/>
-      <c r="I58" s="15"/>
-      <c r="J58" s="15"/>
-      <c r="K58" s="15"/>
-      <c r="L58" s="15"/>
-      <c r="M58" s="15"/>
-      <c r="N58" s="15"/>
-      <c r="O58" s="15"/>
-      <c r="P58" s="15"/>
-    </row>
-    <row r="59" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B59" s="19" t="s">
+      <c r="B58" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C59" s="19" t="s">
+      <c r="C58" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="D59" s="34"/>
-      <c r="E59" s="34" t="s">
+      <c r="D58" s="34"/>
+      <c r="E58" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="F59" s="34"/>
-      <c r="G59" s="34" t="s">
+      <c r="F58" s="34"/>
+      <c r="G58" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="H59" s="34"/>
+      <c r="H58" s="34"/>
+    </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B59" s="35"/>
+      <c r="C59" t="s">
+        <v>159</v>
+      </c>
+      <c r="E59" t="s">
+        <v>50</v>
+      </c>
+      <c r="F59">
+        <v>4539</v>
+      </c>
+      <c r="G59" t="s">
+        <v>264</v>
+      </c>
+      <c r="H59">
+        <v>4539</v>
+      </c>
+      <c r="I59">
+        <v>1</v>
+      </c>
+      <c r="J59">
+        <v>1</v>
+      </c>
+      <c r="K59">
+        <f t="shared" ref="K59" si="18">IF(I59&gt;0,CEILING(I59/J59,1),0)</f>
+        <v>1</v>
+      </c>
+      <c r="L59" s="36">
+        <v>5</v>
+      </c>
+      <c r="M59" s="24">
+        <f>IF(I59&gt;0,L59/J59*I59,0)</f>
+        <v>5</v>
+      </c>
+      <c r="N59" s="32">
+        <f t="shared" ref="N59:N60" si="19">K59*L59</f>
+        <v>5</v>
+      </c>
+      <c r="P59" s="25" t="s">
+        <v>265</v>
+      </c>
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B60" s="35"/>
       <c r="C60" t="s">
-        <v>161</v>
+        <v>266</v>
       </c>
       <c r="E60" t="s">
         <v>50</v>
@@ -4005,51 +3989,50 @@
         <v>4539</v>
       </c>
       <c r="G60" t="s">
+        <v>72</v>
+      </c>
+      <c r="H60" t="s">
+        <v>267</v>
+      </c>
+      <c r="I60">
+        <v>1</v>
+      </c>
+      <c r="J60">
+        <v>1</v>
+      </c>
+      <c r="K60">
+        <v>1</v>
+      </c>
+      <c r="L60" s="11">
+        <v>7.63</v>
+      </c>
+      <c r="M60" s="24">
+        <f t="shared" ref="M60" si="20">IF(I60&gt;0,L60/J60*I60,0)</f>
+        <v>7.63</v>
+      </c>
+      <c r="N60" s="32">
+        <f t="shared" si="19"/>
+        <v>7.63</v>
+      </c>
+      <c r="P60" s="25" t="s">
         <v>268</v>
       </c>
-      <c r="H60">
-        <v>4539</v>
-      </c>
-      <c r="I60">
-        <v>1</v>
-      </c>
-      <c r="J60">
-        <v>1</v>
-      </c>
-      <c r="K60">
-        <f t="shared" ref="K60" si="18">IF(I60&gt;0,CEILING(I60/J60,1),0)</f>
-        <v>1</v>
-      </c>
-      <c r="L60" s="36">
-        <v>5</v>
-      </c>
-      <c r="M60" s="24">
-        <f>IF(I60&gt;0,L60/J60*I60,0)</f>
-        <v>5</v>
-      </c>
-      <c r="N60" s="32">
-        <f t="shared" ref="N60:N61" si="19">K60*L60</f>
-        <v>5</v>
-      </c>
-      <c r="P60" s="25" t="s">
-        <v>269</v>
-      </c>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C61" t="s">
-        <v>270</v>
+      <c r="C61" s="38" t="s">
+        <v>210</v>
       </c>
       <c r="E61" t="s">
         <v>50</v>
       </c>
       <c r="F61">
-        <v>4539</v>
+        <v>2011</v>
       </c>
       <c r="G61" t="s">
-        <v>72</v>
-      </c>
-      <c r="H61" t="s">
-        <v>271</v>
+        <v>264</v>
+      </c>
+      <c r="H61">
+        <v>2011</v>
       </c>
       <c r="I61">
         <v>1</v>
@@ -4061,41 +4044,38 @@
         <v>1</v>
       </c>
       <c r="L61" s="11">
-        <v>7.63</v>
+        <v>12.5</v>
       </c>
       <c r="M61" s="24">
-        <f t="shared" ref="M61" si="20">IF(I61&gt;0,L61/J61*I61,0)</f>
-        <v>7.63</v>
+        <f t="shared" ref="M61" si="21">IF(I61&gt;0,L61/J61*I61,0)</f>
+        <v>12.5</v>
       </c>
       <c r="N61" s="32">
-        <f t="shared" si="19"/>
-        <v>7.63</v>
+        <f t="shared" ref="N61" si="22">K61*L61</f>
+        <v>12.5</v>
       </c>
       <c r="P61" s="25" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>216</v>
+      </c>
       <c r="C62" s="38" t="s">
-        <v>213</v>
-      </c>
-      <c r="E62" t="s">
+        <v>225</v>
+      </c>
+      <c r="G62" t="s">
+        <v>285</v>
+      </c>
+      <c r="H62" s="59" t="s">
+        <v>287</v>
+      </c>
+      <c r="I62">
+        <v>2</v>
+      </c>
+      <c r="J62">
         <v>50</v>
-      </c>
-      <c r="F62">
-        <v>2011</v>
-      </c>
-      <c r="G62" t="s">
-        <v>268</v>
-      </c>
-      <c r="H62">
-        <v>2011</v>
-      </c>
-      <c r="I62">
-        <v>1</v>
-      </c>
-      <c r="J62">
-        <v>1</v>
       </c>
       <c r="K62">
         <v>1</v>
@@ -4104,32 +4084,29 @@
         <v>12.5</v>
       </c>
       <c r="M62" s="24">
-        <f t="shared" ref="M62" si="21">IF(I62&gt;0,L62/J62*I62,0)</f>
+        <f t="shared" ref="M62" si="23">IF(I62&gt;0,L62/J62*I62,0)</f>
+        <v>0.5</v>
+      </c>
+      <c r="N62" s="32">
+        <f t="shared" ref="N62" si="24">K62*L62</f>
         <v>12.5</v>
       </c>
-      <c r="N62" s="32">
-        <f t="shared" ref="N62" si="22">K62*L62</f>
-        <v>12.5</v>
-      </c>
-      <c r="P62" s="25" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="63" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>219</v>
-      </c>
-      <c r="C63" s="38" t="s">
-        <v>228</v>
+        <v>217</v>
+      </c>
+      <c r="C63" s="40" t="s">
+        <v>226</v>
       </c>
       <c r="G63" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
       <c r="H63" s="59" t="s">
-        <v>296</v>
+        <v>286</v>
       </c>
       <c r="I63">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J63">
         <v>50</v>
@@ -4141,69 +4118,69 @@
         <v>12.5</v>
       </c>
       <c r="M63" s="24">
-        <f t="shared" ref="M63" si="23">IF(I63&gt;0,L63/J63*I63,0)</f>
-        <v>0.5</v>
+        <f>IF(I63&gt;0,L63/J63*I63,0)</f>
+        <v>1</v>
       </c>
       <c r="N63" s="32">
-        <f t="shared" ref="N63" si="24">K63*L63</f>
+        <f>K63*L63</f>
         <v>12.5</v>
       </c>
-    </row>
-    <row r="64" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" t="s">
-        <v>220</v>
-      </c>
-      <c r="C64" s="40" t="s">
-        <v>229</v>
+      <c r="P63" s="8" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
+        <v>319</v>
+      </c>
+      <c r="C64" s="38" t="s">
+        <v>312</v>
+      </c>
+      <c r="E64" t="s">
+        <v>313</v>
+      </c>
+      <c r="F64" t="s">
+        <v>314</v>
       </c>
       <c r="G64" t="s">
-        <v>294</v>
-      </c>
-      <c r="H64" s="59" t="s">
-        <v>295</v>
+        <v>72</v>
+      </c>
+      <c r="H64" t="s">
+        <v>315</v>
       </c>
       <c r="I64">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J64">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="K64">
         <v>1</v>
       </c>
       <c r="L64" s="11">
-        <v>12.5</v>
+        <v>12.11</v>
       </c>
       <c r="M64" s="24">
         <f>IF(I64&gt;0,L64/J64*I64,0)</f>
-        <v>1</v>
+        <v>36.33</v>
       </c>
       <c r="N64" s="32">
         <f>K64*L64</f>
-        <v>12.5</v>
+        <v>12.11</v>
       </c>
       <c r="P64" s="8" t="s">
-        <v>297</v>
+        <v>317</v>
       </c>
     </row>
     <row r="65" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>328</v>
-      </c>
-      <c r="C65" s="38" t="s">
-        <v>321</v>
-      </c>
-      <c r="E65" t="s">
-        <v>322</v>
-      </c>
-      <c r="F65" t="s">
-        <v>323</v>
+        <v>319</v>
+      </c>
+      <c r="C65" t="s">
+        <v>318</v>
       </c>
       <c r="G65" t="s">
-        <v>72</v>
-      </c>
-      <c r="H65" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="I65">
         <v>3</v>
@@ -4215,29 +4192,29 @@
         <v>1</v>
       </c>
       <c r="L65" s="11">
-        <v>12.11</v>
-      </c>
-      <c r="M65" s="24">
+        <v>9.9499999999999993</v>
+      </c>
+      <c r="M65" s="61">
         <f>IF(I65&gt;0,L65/J65*I65,0)</f>
-        <v>36.33</v>
-      </c>
-      <c r="N65" s="32">
+        <v>29.849999999999998</v>
+      </c>
+      <c r="N65" s="62">
         <f>K65*L65</f>
-        <v>12.11</v>
+        <v>9.9499999999999993</v>
       </c>
       <c r="P65" s="8" t="s">
-        <v>326</v>
+        <v>316</v>
       </c>
     </row>
     <row r="66" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>328</v>
-      </c>
-      <c r="C66" t="s">
-        <v>327</v>
+        <v>319</v>
+      </c>
+      <c r="C66" s="38" t="s">
+        <v>312</v>
       </c>
       <c r="G66" t="s">
-        <v>329</v>
+        <v>333</v>
       </c>
       <c r="I66">
         <v>3</v>
@@ -4249,29 +4226,30 @@
         <v>1</v>
       </c>
       <c r="L66" s="11">
-        <v>9.9499999999999993</v>
-      </c>
-      <c r="M66" s="62">
+        <v>5</v>
+      </c>
+      <c r="M66" s="24">
         <f>IF(I66&gt;0,L66/J66*I66,0)</f>
-        <v>29.849999999999998</v>
-      </c>
-      <c r="N66" s="63">
+        <v>15</v>
+      </c>
+      <c r="N66" s="32">
         <f>K66*L66</f>
-        <v>9.9499999999999993</v>
-      </c>
-      <c r="P66" s="8" t="s">
-        <v>325</v>
+        <v>5</v>
+      </c>
+      <c r="P66" s="8"/>
+      <c r="Q66" t="s">
+        <v>340</v>
       </c>
     </row>
     <row r="67" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>328</v>
-      </c>
-      <c r="C67" s="38" t="s">
-        <v>321</v>
+        <v>331</v>
+      </c>
+      <c r="C67" t="s">
+        <v>332</v>
       </c>
       <c r="G67" t="s">
-        <v>342</v>
+        <v>333</v>
       </c>
       <c r="I67">
         <v>3</v>
@@ -4283,190 +4261,203 @@
         <v>1</v>
       </c>
       <c r="L67" s="11">
-        <v>5</v>
-      </c>
-      <c r="M67" s="24">
+        <v>1</v>
+      </c>
+      <c r="M67" s="61">
         <f>IF(I67&gt;0,L67/J67*I67,0)</f>
+        <v>3</v>
+      </c>
+      <c r="N67" s="62">
+        <f>K67*L67</f>
+        <v>1</v>
+      </c>
+      <c r="P67" s="8"/>
+    </row>
+    <row r="68" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="18"/>
+      <c r="B68" s="18"/>
+      <c r="C68" s="18"/>
+      <c r="D68" s="18"/>
+      <c r="E68" s="18"/>
+      <c r="F68" s="18"/>
+      <c r="G68" s="18"/>
+      <c r="H68" s="18"/>
+      <c r="I68" s="18"/>
+      <c r="J68" s="18"/>
+      <c r="K68" s="18"/>
+      <c r="L68" s="55">
+        <f>J68/1000*$C$45</f>
+        <v>0</v>
+      </c>
+      <c r="M68" s="55">
+        <f t="shared" ref="M68" si="25">L68</f>
+        <v>0</v>
+      </c>
+      <c r="N68" s="55">
+        <f t="shared" ref="N68" si="26">L68</f>
+        <v>0</v>
+      </c>
+      <c r="O68" s="56"/>
+      <c r="P68" s="18"/>
+    </row>
+    <row r="69" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B69" s="54" t="s">
+        <v>321</v>
+      </c>
+      <c r="C69" s="15"/>
+      <c r="D69" s="15"/>
+      <c r="E69" s="15"/>
+      <c r="F69" s="15"/>
+      <c r="G69" s="15"/>
+      <c r="H69" s="15"/>
+      <c r="I69" s="15">
+        <v>1</v>
+      </c>
+      <c r="J69" s="15"/>
+      <c r="K69" s="15"/>
+      <c r="L69" s="15"/>
+      <c r="M69" s="15"/>
+      <c r="N69" s="15"/>
+      <c r="O69" s="15"/>
+      <c r="P69" s="15"/>
+    </row>
+    <row r="70" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B70" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C70" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D70" s="34"/>
+      <c r="E70" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="F70" s="34"/>
+      <c r="G70" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="N67" s="32">
-        <f>K67*L67</f>
-        <v>5</v>
-      </c>
-      <c r="P67" s="8"/>
-      <c r="Q67" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B68" t="s">
-        <v>340</v>
-      </c>
-      <c r="C68" t="s">
-        <v>341</v>
-      </c>
-      <c r="G68" t="s">
-        <v>342</v>
-      </c>
-      <c r="I68">
-        <v>3</v>
-      </c>
-      <c r="J68">
-        <v>1</v>
-      </c>
-      <c r="K68">
-        <v>1</v>
-      </c>
-      <c r="L68" s="11">
-        <v>1</v>
-      </c>
-      <c r="M68" s="62">
-        <f>IF(I68&gt;0,L68/J68*I68,0)</f>
-        <v>3</v>
-      </c>
-      <c r="N68" s="63">
-        <f>K68*L68</f>
-        <v>1</v>
-      </c>
-      <c r="P68" s="8"/>
-    </row>
-    <row r="69" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="18"/>
-      <c r="B69" s="18"/>
-      <c r="C69" s="18"/>
-      <c r="D69" s="18"/>
-      <c r="E69" s="18"/>
-      <c r="F69" s="18"/>
-      <c r="G69" s="18"/>
-      <c r="H69" s="18"/>
-      <c r="I69" s="18"/>
-      <c r="J69" s="18"/>
-      <c r="K69" s="18"/>
-      <c r="L69" s="55">
-        <f>J69/1000*$C$46</f>
-        <v>0</v>
-      </c>
-      <c r="M69" s="55">
-        <f t="shared" ref="M69" si="25">L69</f>
-        <v>0</v>
-      </c>
-      <c r="N69" s="55">
-        <f t="shared" ref="N69" si="26">L69</f>
-        <v>0</v>
-      </c>
-      <c r="O69" s="56"/>
-      <c r="P69" s="18"/>
-    </row>
-    <row r="70" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B70" s="54" t="s">
-        <v>330</v>
-      </c>
-      <c r="C70" s="15"/>
-      <c r="D70" s="15"/>
-      <c r="E70" s="15"/>
-      <c r="F70" s="15"/>
-      <c r="G70" s="15"/>
-      <c r="H70" s="15"/>
-      <c r="I70" s="15">
-        <v>1</v>
-      </c>
-      <c r="J70" s="15"/>
-      <c r="K70" s="15"/>
-      <c r="L70" s="15"/>
-      <c r="M70" s="15"/>
-      <c r="N70" s="15"/>
-      <c r="O70" s="15"/>
-      <c r="P70" s="15"/>
-    </row>
-    <row r="71" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B71" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="C71" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="D71" s="34"/>
-      <c r="E71" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="F71" s="34"/>
-      <c r="G71" s="34" t="s">
-        <v>15</v>
-      </c>
-      <c r="H71" s="34"/>
+      <c r="H70" s="34"/>
+    </row>
+    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>245</v>
+      </c>
+      <c r="B71" t="s">
+        <v>127</v>
+      </c>
+      <c r="C71" t="s">
+        <v>110</v>
+      </c>
+      <c r="E71" t="s">
+        <v>100</v>
+      </c>
+      <c r="F71" t="s">
+        <v>83</v>
+      </c>
+      <c r="G71" t="s">
+        <v>72</v>
+      </c>
+      <c r="H71" t="s">
+        <v>144</v>
+      </c>
+      <c r="I71">
+        <f>I69*1</f>
+        <v>1</v>
+      </c>
+      <c r="J71">
+        <v>1</v>
+      </c>
+      <c r="K71" s="23">
+        <f t="shared" ref="K71:K87" si="27">IF(I71&gt;0,CEILING(I71/J71,1),0)</f>
+        <v>1</v>
+      </c>
+      <c r="L71" s="11">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="M71" s="24">
+        <f t="shared" ref="M71:M87" si="28">IF(I71&gt;0,L71/J71*I71,0)</f>
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="N71" s="24">
+        <f t="shared" ref="N71:N87" si="29">K71*L71</f>
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="P71" s="25" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="72" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="B72" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C72" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E72" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F72" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="G72" t="s">
         <v>72</v>
       </c>
       <c r="H72" t="s">
-        <v>144</v>
+        <v>177</v>
       </c>
       <c r="I72">
-        <f>I70*1</f>
-        <v>1</v>
+        <f t="shared" ref="I72:I76" si="30">$I$22*1</f>
+        <v>3</v>
       </c>
       <c r="J72">
         <v>1</v>
       </c>
       <c r="K72" s="23">
-        <f t="shared" ref="K72:K88" si="27">IF(I72&gt;0,CEILING(I72/J72,1),0)</f>
-        <v>1</v>
+        <f t="shared" si="27"/>
+        <v>3</v>
       </c>
       <c r="L72" s="11">
-        <v>1.1200000000000001</v>
+        <v>2.68</v>
       </c>
       <c r="M72" s="24">
-        <f t="shared" ref="M72:M88" si="28">IF(I72&gt;0,L72/J72*I72,0)</f>
-        <v>1.1200000000000001</v>
+        <f t="shared" si="28"/>
+        <v>8.0400000000000009</v>
       </c>
       <c r="N72" s="24">
-        <f t="shared" ref="N72:N88" si="29">K72*L72</f>
-        <v>1.1200000000000001</v>
+        <f t="shared" si="29"/>
+        <v>8.0400000000000009</v>
       </c>
       <c r="P72" s="25" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="73" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="B73" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C73" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E73" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F73" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G73" t="s">
         <v>72</v>
       </c>
       <c r="H73" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I73">
-        <f t="shared" ref="I73:I77" si="30">$I$22*1</f>
+        <f t="shared" si="30"/>
         <v>3</v>
       </c>
       <c r="J73">
@@ -4477,41 +4468,41 @@
         <v>3</v>
       </c>
       <c r="L73" s="11">
-        <v>2.68</v>
+        <v>1.46</v>
       </c>
       <c r="M73" s="24">
         <f t="shared" si="28"/>
-        <v>8.0400000000000009</v>
+        <v>4.38</v>
       </c>
       <c r="N73" s="24">
         <f t="shared" si="29"/>
-        <v>8.0400000000000009</v>
+        <v>4.38</v>
       </c>
       <c r="P73" s="25" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="74" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="B74" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C74" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E74" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="F74" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="G74" t="s">
         <v>72</v>
       </c>
       <c r="H74" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I74">
         <f t="shared" si="30"/>
@@ -4525,41 +4516,41 @@
         <v>3</v>
       </c>
       <c r="L74" s="11">
-        <v>1.46</v>
+        <v>7.32</v>
       </c>
       <c r="M74" s="24">
         <f t="shared" si="28"/>
-        <v>4.38</v>
+        <v>21.96</v>
       </c>
       <c r="N74" s="24">
         <f t="shared" si="29"/>
-        <v>4.38</v>
+        <v>21.96</v>
       </c>
       <c r="P74" s="25" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="75" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="B75" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C75" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E75" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F75" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G75" t="s">
         <v>72</v>
       </c>
       <c r="H75" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I75">
         <f t="shared" si="30"/>
@@ -4573,41 +4564,41 @@
         <v>3</v>
       </c>
       <c r="L75" s="11">
-        <v>7.32</v>
+        <v>0.6</v>
       </c>
       <c r="M75" s="24">
         <f t="shared" si="28"/>
-        <v>21.96</v>
+        <v>1.7999999999999998</v>
       </c>
       <c r="N75" s="24">
         <f t="shared" si="29"/>
-        <v>21.96</v>
-      </c>
-      <c r="P75" s="25" t="s">
-        <v>165</v>
+        <v>1.7999999999999998</v>
+      </c>
+      <c r="P75" s="8" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="76" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="B76" t="s">
-        <v>131</v>
+        <v>78</v>
       </c>
       <c r="C76" t="s">
-        <v>114</v>
+        <v>41</v>
       </c>
       <c r="E76" t="s">
-        <v>104</v>
+        <v>49</v>
       </c>
       <c r="F76" t="s">
-        <v>87</v>
+        <v>59</v>
       </c>
       <c r="G76" t="s">
         <v>72</v>
       </c>
       <c r="H76" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="I76">
         <f t="shared" si="30"/>
@@ -4621,185 +4612,185 @@
         <v>3</v>
       </c>
       <c r="L76" s="11">
-        <v>0.6</v>
+        <v>0.91</v>
       </c>
       <c r="M76" s="24">
         <f t="shared" si="28"/>
-        <v>1.7999999999999998</v>
+        <v>2.73</v>
       </c>
       <c r="N76" s="24">
         <f t="shared" si="29"/>
-        <v>1.7999999999999998</v>
-      </c>
-      <c r="P76" s="8" t="s">
-        <v>165</v>
+        <v>2.73</v>
+      </c>
+      <c r="P76" s="25" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="77" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="B77" t="s">
-        <v>78</v>
+        <v>132</v>
       </c>
       <c r="C77" t="s">
-        <v>41</v>
+        <v>115</v>
       </c>
       <c r="E77" t="s">
-        <v>49</v>
+        <v>105</v>
       </c>
       <c r="F77" t="s">
-        <v>59</v>
+        <v>88</v>
       </c>
       <c r="G77" t="s">
         <v>72</v>
       </c>
       <c r="H77" t="s">
-        <v>183</v>
+        <v>145</v>
       </c>
       <c r="I77">
-        <f t="shared" si="30"/>
-        <v>3</v>
+        <f>$I$22*3</f>
+        <v>9</v>
       </c>
       <c r="J77">
         <v>1</v>
       </c>
       <c r="K77" s="23">
         <f t="shared" si="27"/>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="L77" s="11">
-        <v>0.91</v>
+        <v>0.15</v>
       </c>
       <c r="M77" s="24">
         <f t="shared" si="28"/>
-        <v>2.73</v>
+        <v>1.3499999999999999</v>
       </c>
       <c r="N77" s="24">
         <f t="shared" si="29"/>
-        <v>2.73</v>
-      </c>
-      <c r="P77" s="25" t="s">
-        <v>153</v>
+        <v>1.3499999999999999</v>
+      </c>
+      <c r="P77" s="8" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="B78" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C78" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E78" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F78" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="G78" t="s">
         <v>72</v>
       </c>
       <c r="H78" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="I78">
-        <f>$I$22*3</f>
-        <v>9</v>
+        <f>$I$22*5</f>
+        <v>15</v>
       </c>
       <c r="J78">
         <v>1</v>
       </c>
       <c r="K78" s="23">
         <f t="shared" si="27"/>
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="L78" s="11">
         <v>0.15</v>
       </c>
       <c r="M78" s="24">
         <f t="shared" si="28"/>
-        <v>1.3499999999999999</v>
+        <v>2.25</v>
       </c>
       <c r="N78" s="24">
         <f t="shared" si="29"/>
-        <v>1.3499999999999999</v>
-      </c>
-      <c r="P78" s="8" t="s">
-        <v>166</v>
+        <v>2.25</v>
+      </c>
+      <c r="P78" s="25" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="79" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="B79" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C79" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E79" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F79" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="G79" t="s">
         <v>72</v>
       </c>
       <c r="H79" t="s">
-        <v>146</v>
+        <v>176</v>
       </c>
       <c r="I79">
-        <f>$I$22*5</f>
-        <v>15</v>
+        <f>$I$22*1</f>
+        <v>3</v>
       </c>
       <c r="J79">
         <v>1</v>
       </c>
       <c r="K79" s="23">
         <f t="shared" si="27"/>
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="L79" s="11">
-        <v>0.15</v>
+        <v>0.47</v>
       </c>
       <c r="M79" s="24">
         <f t="shared" si="28"/>
-        <v>2.25</v>
+        <v>1.41</v>
       </c>
       <c r="N79" s="24">
         <f t="shared" si="29"/>
-        <v>2.25</v>
+        <v>1.41</v>
       </c>
       <c r="P79" s="25" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="80" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="B80" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C80" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E80" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F80" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="G80" t="s">
         <v>72</v>
       </c>
       <c r="H80" t="s">
-        <v>178</v>
+        <v>147</v>
       </c>
       <c r="I80">
         <f>$I$22*1</f>
@@ -4813,41 +4804,41 @@
         <v>3</v>
       </c>
       <c r="L80" s="11">
-        <v>0.47</v>
+        <v>0.16</v>
       </c>
       <c r="M80" s="24">
         <f t="shared" si="28"/>
-        <v>1.41</v>
+        <v>0.48</v>
       </c>
       <c r="N80" s="24">
         <f t="shared" si="29"/>
-        <v>1.41</v>
+        <v>0.48</v>
       </c>
       <c r="P80" s="25" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="81" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="B81" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C81" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E81" t="s">
         <v>108</v>
       </c>
       <c r="F81" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G81" t="s">
         <v>72</v>
       </c>
       <c r="H81" t="s">
-        <v>147</v>
+        <v>182</v>
       </c>
       <c r="I81">
         <f>$I$22*1</f>
@@ -4872,126 +4863,126 @@
         <v>0.48</v>
       </c>
       <c r="P81" s="25" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="82" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="B82" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C82" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E82" t="s">
         <v>108</v>
       </c>
       <c r="F82" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G82" t="s">
         <v>72</v>
       </c>
       <c r="H82" t="s">
+        <v>183</v>
+      </c>
+      <c r="I82">
+        <f>$I$22*2</f>
+        <v>6</v>
+      </c>
+      <c r="J82">
+        <v>1</v>
+      </c>
+      <c r="K82" s="23">
+        <f t="shared" si="27"/>
+        <v>6</v>
+      </c>
+      <c r="L82" s="11">
+        <v>0.16</v>
+      </c>
+      <c r="M82" s="24">
+        <f t="shared" si="28"/>
+        <v>0.96</v>
+      </c>
+      <c r="N82" s="24">
+        <f t="shared" si="29"/>
+        <v>0.96</v>
+      </c>
+      <c r="P82" s="25" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>257</v>
+      </c>
+      <c r="B83" t="s">
+        <v>138</v>
+      </c>
+      <c r="C83" t="s">
+        <v>121</v>
+      </c>
+      <c r="E83" t="s">
+        <v>108</v>
+      </c>
+      <c r="F83" t="s">
+        <v>94</v>
+      </c>
+      <c r="G83" t="s">
+        <v>72</v>
+      </c>
+      <c r="H83" t="s">
         <v>184</v>
       </c>
-      <c r="I82">
+      <c r="I83">
         <f>$I$22*1</f>
         <v>3</v>
       </c>
-      <c r="J82">
-        <v>1</v>
-      </c>
-      <c r="K82" s="23">
+      <c r="J83">
+        <v>1</v>
+      </c>
+      <c r="K83" s="23">
         <f t="shared" si="27"/>
         <v>3</v>
       </c>
-      <c r="L82" s="11">
+      <c r="L83" s="11">
         <v>0.16</v>
       </c>
-      <c r="M82" s="24">
+      <c r="M83" s="24">
         <f t="shared" si="28"/>
         <v>0.48</v>
       </c>
-      <c r="N82" s="24">
+      <c r="N83" s="24">
         <f t="shared" si="29"/>
         <v>0.48</v>
       </c>
-      <c r="P82" s="25" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>260</v>
-      </c>
-      <c r="B83" t="s">
-        <v>137</v>
-      </c>
-      <c r="C83" t="s">
-        <v>120</v>
-      </c>
-      <c r="E83" t="s">
-        <v>108</v>
-      </c>
-      <c r="F83" t="s">
-        <v>93</v>
-      </c>
-      <c r="G83" t="s">
-        <v>72</v>
-      </c>
-      <c r="H83" t="s">
-        <v>185</v>
-      </c>
-      <c r="I83">
-        <f>$I$22*2</f>
-        <v>6</v>
-      </c>
-      <c r="J83">
-        <v>1</v>
-      </c>
-      <c r="K83" s="23">
-        <f t="shared" si="27"/>
-        <v>6</v>
-      </c>
-      <c r="L83" s="11">
-        <v>0.16</v>
-      </c>
-      <c r="M83" s="24">
-        <f t="shared" si="28"/>
-        <v>0.96</v>
-      </c>
-      <c r="N83" s="24">
-        <f t="shared" si="29"/>
-        <v>0.96</v>
-      </c>
       <c r="P83" s="25" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="84" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="B84" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C84" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E84" t="s">
         <v>108</v>
       </c>
       <c r="F84" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="G84" t="s">
         <v>72</v>
       </c>
       <c r="H84" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I84">
         <f>$I$22*1</f>
@@ -5016,30 +5007,30 @@
         <v>0.48</v>
       </c>
       <c r="P84" s="25" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="85" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="B85" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C85" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E85" t="s">
         <v>108</v>
       </c>
       <c r="F85" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G85" t="s">
         <v>72</v>
       </c>
       <c r="H85" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="I85">
         <f>$I$22*1</f>
@@ -5064,164 +5055,116 @@
         <v>0.48</v>
       </c>
       <c r="P85" s="25" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="86" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="B86" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C86" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E86" t="s">
         <v>108</v>
       </c>
       <c r="F86" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="G86" t="s">
         <v>72</v>
       </c>
       <c r="H86" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I86">
         <f>$I$22*1</f>
         <v>3</v>
       </c>
       <c r="J86">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="K86" s="23">
         <f t="shared" si="27"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L86" s="11">
         <v>0.16</v>
       </c>
       <c r="M86" s="24">
         <f t="shared" si="28"/>
-        <v>0.48</v>
+        <v>9.6000000000000002E-2</v>
       </c>
       <c r="N86" s="24">
         <f t="shared" si="29"/>
-        <v>0.48</v>
+        <v>0.16</v>
       </c>
       <c r="P86" s="25" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="87" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="B87" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C87" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E87" t="s">
         <v>108</v>
       </c>
       <c r="F87" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G87" t="s">
         <v>72</v>
       </c>
       <c r="H87" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="I87">
-        <f>$I$22*1</f>
-        <v>3</v>
+        <f>$I$22*2</f>
+        <v>6</v>
       </c>
       <c r="J87">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="K87" s="23">
         <f t="shared" si="27"/>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="L87" s="11">
         <v>0.16</v>
       </c>
       <c r="M87" s="24">
         <f t="shared" si="28"/>
-        <v>9.6000000000000002E-2</v>
+        <v>0.96</v>
       </c>
       <c r="N87" s="24">
         <f t="shared" si="29"/>
-        <v>0.16</v>
+        <v>0.96</v>
       </c>
       <c r="P87" s="25" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
-        <v>265</v>
-      </c>
-      <c r="B88" t="s">
-        <v>142</v>
-      </c>
-      <c r="C88" t="s">
-        <v>125</v>
-      </c>
-      <c r="E88" t="s">
-        <v>108</v>
-      </c>
-      <c r="F88" t="s">
-        <v>98</v>
-      </c>
-      <c r="G88" t="s">
-        <v>72</v>
-      </c>
-      <c r="H88" t="s">
-        <v>190</v>
-      </c>
-      <c r="I88">
-        <f>$I$22*2</f>
-        <v>6</v>
-      </c>
-      <c r="J88">
-        <v>1</v>
-      </c>
-      <c r="K88" s="23">
-        <f t="shared" si="27"/>
-        <v>6</v>
-      </c>
-      <c r="L88" s="11">
-        <v>0.16</v>
-      </c>
-      <c r="M88" s="24">
-        <f t="shared" si="28"/>
-        <v>0.96</v>
-      </c>
-      <c r="N88" s="24">
-        <f t="shared" si="29"/>
-        <v>0.96</v>
-      </c>
-      <c r="P88" s="25" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="98" spans="13:13" x14ac:dyDescent="0.25">
-      <c r="M98" s="20"/>
+        <v>169</v>
+      </c>
+    </row>
+    <row r="97" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M97" s="20"/>
+    </row>
+    <row r="100" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M100" s="20"/>
     </row>
     <row r="101" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M101" s="20"/>
     </row>
-    <row r="102" spans="13:13" x14ac:dyDescent="0.25">
-      <c r="M102" s="20"/>
-    </row>
-    <row r="106" spans="13:13" x14ac:dyDescent="0.25">
-      <c r="M106" s="20"/>
+    <row r="105" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M105" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -5233,8 +5176,8 @@
   </mergeCells>
   <phoneticPr fontId="14" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="P78" r:id="rId1" xr:uid="{60E6A92C-4839-489E-AD1E-F1DD2C496A62}"/>
-    <hyperlink ref="P76" r:id="rId2" xr:uid="{5AB49DB6-CF7A-4FB5-9BF1-A6DF95EDC91C}"/>
+    <hyperlink ref="P77" r:id="rId1" xr:uid="{60E6A92C-4839-489E-AD1E-F1DD2C496A62}"/>
+    <hyperlink ref="P75" r:id="rId2" xr:uid="{5AB49DB6-CF7A-4FB5-9BF1-A6DF95EDC91C}"/>
     <hyperlink ref="P11" r:id="rId3" xr:uid="{98E71B01-F4EE-404B-8A84-09D2B5DC23E0}"/>
     <hyperlink ref="P6" r:id="rId4" xr:uid="{9691E2C5-8C3E-4DFF-A8CF-17294451BFA1}"/>
     <hyperlink ref="P7" r:id="rId5" xr:uid="{4027CBE2-8F4B-4B3C-9C92-54C41274035F}"/>
@@ -5249,17 +5192,17 @@
     <hyperlink ref="P16" r:id="rId14" xr:uid="{0BAD0BDA-91BD-4AF4-AB9F-7D0701EDC500}"/>
     <hyperlink ref="P24" r:id="rId15" xr:uid="{CA86E1D3-1641-48F6-8990-E8A7041B7767}"/>
     <hyperlink ref="P25" r:id="rId16" xr:uid="{0EBD983D-EF23-4E50-B944-9B75B3417064}"/>
-    <hyperlink ref="P33" r:id="rId17" xr:uid="{60B810BC-D3B0-44AC-8984-679B3FFFCE28}"/>
-    <hyperlink ref="P32" r:id="rId18" xr:uid="{E4E91C58-5C72-4626-BFC1-B08D53B102A0}"/>
-    <hyperlink ref="P64" r:id="rId19" xr:uid="{C9EF98AB-74D8-4339-B9CC-AABB9586DAD3}"/>
-    <hyperlink ref="P14" r:id="rId20" xr:uid="{5CD1FACD-C73A-4FC4-8C13-6A315EE91F2C}"/>
-    <hyperlink ref="P36" r:id="rId21" xr:uid="{D6CF539C-D7A9-4DF6-A152-90C647EDF6C0}"/>
-    <hyperlink ref="P37" r:id="rId22" xr:uid="{BE1FCFA9-E21B-4476-8C60-6567B7F119AC}"/>
-    <hyperlink ref="P28" r:id="rId23" xr:uid="{13B8A810-4A35-4DFB-A533-5BF3750957DB}"/>
-    <hyperlink ref="P27" r:id="rId24" xr:uid="{27565B5C-C6CB-475E-B49B-8DCC28094257}"/>
-    <hyperlink ref="P65" r:id="rId25" xr:uid="{10EF546D-8F3B-4FA5-B77B-77DBB0886554}"/>
-    <hyperlink ref="P66" r:id="rId26" xr:uid="{BD0BC4D2-7507-4F5F-B81A-B55D478DB3BB}"/>
-    <hyperlink ref="P30" r:id="rId27" xr:uid="{4B090432-2539-495F-A038-C61EDFAC4B5C}"/>
+    <hyperlink ref="P32" r:id="rId17" xr:uid="{E4E91C58-5C72-4626-BFC1-B08D53B102A0}"/>
+    <hyperlink ref="P63" r:id="rId18" xr:uid="{C9EF98AB-74D8-4339-B9CC-AABB9586DAD3}"/>
+    <hyperlink ref="P14" r:id="rId19" xr:uid="{5CD1FACD-C73A-4FC4-8C13-6A315EE91F2C}"/>
+    <hyperlink ref="P35" r:id="rId20" xr:uid="{D6CF539C-D7A9-4DF6-A152-90C647EDF6C0}"/>
+    <hyperlink ref="P36" r:id="rId21" xr:uid="{BE1FCFA9-E21B-4476-8C60-6567B7F119AC}"/>
+    <hyperlink ref="P28" r:id="rId22" xr:uid="{13B8A810-4A35-4DFB-A533-5BF3750957DB}"/>
+    <hyperlink ref="P27" r:id="rId23" xr:uid="{27565B5C-C6CB-475E-B49B-8DCC28094257}"/>
+    <hyperlink ref="P64" r:id="rId24" xr:uid="{10EF546D-8F3B-4FA5-B77B-77DBB0886554}"/>
+    <hyperlink ref="P65" r:id="rId25" xr:uid="{BD0BC4D2-7507-4F5F-B81A-B55D478DB3BB}"/>
+    <hyperlink ref="P30" r:id="rId26" xr:uid="{4B090432-2539-495F-A038-C61EDFAC4B5C}"/>
+    <hyperlink ref="P33" r:id="rId27" xr:uid="{4F41C6F3-1E43-4053-A223-7226FD49FF85}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId28"/>
@@ -5551,10 +5494,16 @@
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4958292-C6C4-482B-887A-6CF9FB19AB74}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="e718a8af-5d48-45b1-a7fb-cef00c107a7a"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="715913e6-4bf0-458f-8160-f18e142d04ff"/>
-    <ds:schemaRef ds:uri="e718a8af-5d48-45b1-a7fb-cef00c107a7a"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>